<commit_message>
Added staff directory upload section
</commit_message>
<xml_diff>
--- a/formats/getto_format_download.xlsx
+++ b/formats/getto_format_download.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fletch/Desktop/bluffs_getto/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94921ED0-2A7B-8642-A636-BFB34209D91E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="47">
   <si>
     <t>Activity</t>
   </si>
@@ -61,9 +67,6 @@
     <t xml:space="preserve">Ropes </t>
   </si>
   <si>
-    <t>Lifegaurd</t>
-  </si>
-  <si>
     <t>Speaker Snack</t>
   </si>
   <si>
@@ -73,9 +76,6 @@
     <t>Skeet</t>
   </si>
   <si>
-    <t>PPP Lifegaurd</t>
-  </si>
-  <si>
     <t>Blob Spotter</t>
   </si>
   <si>
@@ -130,16 +130,19 @@
     <t>Female</t>
   </si>
   <si>
-    <t>Ropes, Workcrew</t>
-  </si>
-  <si>
-    <t>Lifegaurd, Workcrew</t>
-  </si>
-  <si>
-    <t>Workcrew</t>
-  </si>
-  <si>
-    <t>Male, Workcrew</t>
+    <t>Ropes, Non-program</t>
+  </si>
+  <si>
+    <t>Lifeguard, Non-program</t>
+  </si>
+  <si>
+    <t>Non-program</t>
+  </si>
+  <si>
+    <t>Male, Non-program</t>
+  </si>
+  <si>
+    <t>Female, Non-program</t>
   </si>
   <si>
     <t xml:space="preserve">Male </t>
@@ -149,13 +152,22 @@
   </si>
   <si>
     <t>Leadership, Male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lifeguard </t>
+  </si>
+  <si>
+    <t>Lifeguard , Non-program</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PPP Lifeguard </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,13 +230,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -262,7 +282,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -296,6 +316,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -330,9 +351,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -505,14 +527,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -544,7 +568,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -555,7 +579,7 @@
         <v>800</v>
       </c>
       <c r="E2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -573,7 +597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -602,7 +626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -631,7 +655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -660,7 +684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -671,7 +695,7 @@
         <v>830</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -692,7 +716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -703,7 +727,7 @@
         <v>830</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -724,7 +748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -753,7 +777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -764,7 +788,7 @@
         <v>1200</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
@@ -785,7 +809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -796,7 +820,7 @@
         <v>1200</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -817,9 +841,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B11">
         <v>945</v>
@@ -828,7 +852,7 @@
         <v>1045</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -849,9 +873,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B12">
         <v>945</v>
@@ -860,7 +884,7 @@
         <v>1045</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
@@ -881,9 +905,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B13">
         <v>945</v>
@@ -892,7 +916,7 @@
         <v>1030</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
@@ -913,9 +937,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B14">
         <v>945</v>
@@ -924,7 +948,7 @@
         <v>1030</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
@@ -945,9 +969,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B15">
         <v>1030</v>
@@ -956,7 +980,7 @@
         <v>1145</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
@@ -977,9 +1001,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B16">
         <v>1030</v>
@@ -988,7 +1012,7 @@
         <v>1145</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
@@ -1009,9 +1033,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>1000</v>
@@ -1020,7 +1044,7 @@
         <v>1130</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
@@ -1041,9 +1065,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18">
         <v>1000</v>
@@ -1052,7 +1076,7 @@
         <v>1130</v>
       </c>
       <c r="D18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
@@ -1073,9 +1097,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19">
         <v>1230</v>
@@ -1102,9 +1126,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20">
         <v>1330</v>
@@ -1113,7 +1137,7 @@
         <v>1530</v>
       </c>
       <c r="D20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E20" t="b">
         <v>0</v>
@@ -1134,9 +1158,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21">
         <v>1330</v>
@@ -1145,7 +1169,7 @@
         <v>1530</v>
       </c>
       <c r="D21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
@@ -1166,9 +1190,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="B22">
         <v>1200</v>
@@ -1177,7 +1201,7 @@
         <v>1345</v>
       </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E22" t="b">
         <v>0</v>
@@ -1198,9 +1222,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="B23">
         <v>1200</v>
@@ -1209,7 +1233,7 @@
         <v>1345</v>
       </c>
       <c r="D23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E23" t="b">
         <v>0</v>
@@ -1230,9 +1254,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B24">
         <v>1345</v>
@@ -1241,7 +1265,7 @@
         <v>1515</v>
       </c>
       <c r="D24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E24" t="b">
         <v>0</v>
@@ -1262,9 +1286,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B25">
         <v>1345</v>
@@ -1273,7 +1297,7 @@
         <v>1515</v>
       </c>
       <c r="D25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E25" t="b">
         <v>0</v>
@@ -1294,9 +1318,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B26">
         <v>1500</v>
@@ -1305,7 +1329,7 @@
         <v>1600</v>
       </c>
       <c r="D26" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="E26" t="b">
         <v>1</v>
@@ -1326,9 +1350,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B27">
         <v>1500</v>
@@ -1337,7 +1361,7 @@
         <v>1600</v>
       </c>
       <c r="D27" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="E27" t="b">
         <v>1</v>
@@ -1358,9 +1382,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B28">
         <v>1600</v>
@@ -1369,7 +1393,7 @@
         <v>1700</v>
       </c>
       <c r="D28" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="E28" t="b">
         <v>1</v>
@@ -1390,9 +1414,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B29">
         <v>1600</v>
@@ -1401,7 +1425,7 @@
         <v>1700</v>
       </c>
       <c r="D29" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="E29" t="b">
         <v>1</v>
@@ -1422,9 +1446,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B30">
         <v>1600</v>
@@ -1433,7 +1457,7 @@
         <v>1700</v>
       </c>
       <c r="D30" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="E30" t="b">
         <v>0</v>
@@ -1454,9 +1478,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B31">
         <v>1500</v>
@@ -1483,9 +1507,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B32">
         <v>1600</v>
@@ -1512,9 +1536,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B33">
         <v>1445</v>
@@ -1523,7 +1547,7 @@
         <v>1630</v>
       </c>
       <c r="D33" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E33" t="b">
         <v>0</v>
@@ -1544,9 +1568,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B34">
         <v>1450</v>
@@ -1555,7 +1579,7 @@
         <v>1600</v>
       </c>
       <c r="D34" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E34" t="b">
         <v>0</v>
@@ -1576,9 +1600,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B35">
         <v>1450</v>
@@ -1587,7 +1611,7 @@
         <v>1600</v>
       </c>
       <c r="D35" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E35" t="b">
         <v>0</v>
@@ -1608,9 +1632,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B36">
         <v>1600</v>
@@ -1619,7 +1643,7 @@
         <v>1700</v>
       </c>
       <c r="D36" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E36" t="b">
         <v>0</v>
@@ -1640,9 +1664,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B37">
         <v>1530</v>
@@ -1669,9 +1693,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B38">
         <v>1530</v>
@@ -1698,9 +1722,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B39">
         <v>1530</v>
@@ -1727,9 +1751,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B40">
         <v>1530</v>
@@ -1756,7 +1780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -1788,7 +1812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -1820,7 +1844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -1852,7 +1876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -1884,7 +1908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -1916,7 +1940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -1948,9 +1972,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B47">
         <v>1530</v>
@@ -1959,7 +1983,7 @@
         <v>1700</v>
       </c>
       <c r="D47" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E47" t="b">
         <v>0</v>
@@ -1980,9 +2004,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B48">
         <v>1530</v>
@@ -1991,7 +2015,7 @@
         <v>1700</v>
       </c>
       <c r="D48" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E48" t="b">
         <v>0</v>
@@ -2012,7 +2036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -2023,7 +2047,7 @@
         <v>1600</v>
       </c>
       <c r="D49" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E49" t="b">
         <v>0</v>
@@ -2044,9 +2068,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B50">
         <v>1600</v>
@@ -2055,7 +2079,7 @@
         <v>1700</v>
       </c>
       <c r="D50" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E50" t="b">
         <v>0</v>
@@ -2076,9 +2100,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B51">
         <v>1600</v>
@@ -2087,7 +2111,7 @@
         <v>1700</v>
       </c>
       <c r="D51" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E51" t="b">
         <v>0</v>
@@ -2108,9 +2132,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B52">
         <v>1600</v>
@@ -2119,7 +2143,7 @@
         <v>1700</v>
       </c>
       <c r="D52" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E52" t="b">
         <v>0</v>
@@ -2140,9 +2164,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B53">
         <v>600</v>
@@ -2169,9 +2193,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B54">
         <v>1930</v>
@@ -2180,7 +2204,7 @@
         <v>2030</v>
       </c>
       <c r="D54" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="E54" t="b">
         <v>0</v>
@@ -2201,9 +2225,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B55">
         <v>1930</v>
@@ -2212,7 +2236,7 @@
         <v>2030</v>
       </c>
       <c r="D55" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="E55" t="b">
         <v>0</v>
@@ -2233,9 +2257,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B56">
         <v>2100</v>
@@ -2244,7 +2268,7 @@
         <v>2200</v>
       </c>
       <c r="D56" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="E56" t="b">
         <v>1</v>
@@ -2265,9 +2289,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B57">
         <v>2100</v>
@@ -2276,7 +2300,7 @@
         <v>2200</v>
       </c>
       <c r="D57" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="E57" t="b">
         <v>1</v>
@@ -2297,9 +2321,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B58">
         <v>2100</v>
@@ -2308,7 +2332,7 @@
         <v>2200</v>
       </c>
       <c r="D58" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="E58" t="b">
         <v>1</v>
@@ -2329,9 +2353,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B59">
         <v>2100</v>
@@ -2358,9 +2382,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B60">
         <v>2100</v>
@@ -2387,9 +2411,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B61">
         <v>2300</v>
@@ -2398,7 +2422,7 @@
         <v>2345</v>
       </c>
       <c r="D61" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E61" t="b">
         <v>1</v>
@@ -2419,9 +2443,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B62">
         <v>2300</v>
@@ -2430,7 +2454,7 @@
         <v>2345</v>
       </c>
       <c r="D62" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E62" t="b">
         <v>1</v>

</xml_diff>